<commit_message>
ran chi square in Excel, updated how-to.pptx
</commit_message>
<xml_diff>
--- a/CAH - Client Deck.xlsx
+++ b/CAH - Client Deck.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Documents\2025-CAH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54F7CB4-0D5C-49BA-8CFA-FF5ED6184AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603FD6DB-04C3-40F4-990B-B6A41A9360F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9420" yWindow="825" windowWidth="17130" windowHeight="16350" activeTab="2" xr2:uid="{E6C777D7-8471-4808-94F9-08E8A9949A4A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{E6C777D7-8471-4808-94F9-08E8A9949A4A}"/>
   </bookViews>
   <sheets>
     <sheet name="dumbbell" sheetId="1" r:id="rId1"/>
     <sheet name="donut" sheetId="2" r:id="rId2"/>
-    <sheet name="contingency" sheetId="3" r:id="rId3"/>
+    <sheet name="heatmap" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Before</t>
   </si>
@@ -56,6 +56,48 @@
   </si>
   <si>
     <t>Prior campaigns</t>
+  </si>
+  <si>
+    <t>Excel</t>
+  </si>
+  <si>
+    <t>PowerBI</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Set up project</t>
+  </si>
+  <si>
+    <t>See raw data for diagnosis</t>
+  </si>
+  <si>
+    <t>Factor variables</t>
+  </si>
+  <si>
+    <t>Remove empty rows</t>
+  </si>
+  <si>
+    <t>Filter/Select rows</t>
+  </si>
+  <si>
+    <t>Subset columns</t>
+  </si>
+  <si>
+    <t>Merge data</t>
+  </si>
+  <si>
+    <t>Document/Replicate data cleaning process</t>
+  </si>
+  <si>
+    <t>Descriptive stats, Cross-tabs, Pivot tables</t>
+  </si>
+  <si>
+    <t>Visualize data</t>
+  </si>
+  <si>
+    <t>Run statistical tests</t>
   </si>
 </sst>
 </file>
@@ -4127,14 +4169,192 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF4B734-B75F-4CF0-8321-1BF8290B09CF}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B3:D13">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>